<commit_message>
Additional fixes and updated error guide
</commit_message>
<xml_diff>
--- a/vera/error_guide.xlsx
+++ b/vera/error_guide.xlsx
@@ -29,145 +29,69 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>Line 4: int main(int argc, char** argv) 
-{
-    int res = -1;
-    int stackArray[ 100 ] = { 0 };
-    if (stackArray[ argc+ 100 ])  // BOOM Stack-buffer-overflow
-    {
-         res = 1; 
-    }
-    return res;
-}</t>
-  </si>
-  <si>
-    <t>sanitizer_address-stack_buffer_overflow.c:12: [#1]: Stack buffer overflow, suspect variables: ['stackArray']
- Was accessed by read of size 4 at:
-  sanitizer_address-stack_buffer_overflow.c:8 in function 'main'
- Accessed address is located in stack of thread T0 at offset 692 in frame:
-  sanitizer_address-stack_buffer_overflow.c:5 in function 'main'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">גלישת זיכרון מחסנית, משתנה חשוד ['stackArray']
-הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
-[קובץ] שורה 8 בפונקציה 'main'
-הכתובת המבוקשת ממוקמת במחסנית של חוט T0 בהיסט של 692 בתים במסגרת:
-[קובץ] שורה 5 בפונקציה 'main'   </t>
-  </si>
-  <si>
-    <t>Line 6: int main(void) 
-{ 
- char* p; 
- p[ 100 ] = 'a';
- printf("\n %s \n", p); 
- return 0; 
-}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">גישה לא חוקית לזיכרון (אין הרשאת גישה) - שגיאת סגמנטציה, משתנה חשוד ['p'] ב:
-[קובץ] שורה 9 בפונקציה 'main'
-</t>
-  </si>
-  <si>
-    <t>גלישת זיכרון ערימה, משתנה חשוד ['array']
-הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
-[קובץ] שורה 9 בפונקציה 'main'
-הכתובת המבוקשת ממוקמת 4 בתים מימין לאיזור זיכרון בגודל 400-בתים, שהוקצה ב:
-[קובץ] שורה 7 בפונקציה 'main'</t>
-  </si>
-  <si>
-    <t>Line 3: int globalArray[ 100 ] = {-1 };
-int main(int argc, char** argv) 
-{
-     int res = -1;
-     if (globalArray[ argc+ 100 ]) // BOOM Global-buffer-overflow
-     {
-          res = 1; 
-     }
-     return res;
-}</t>
-  </si>
-  <si>
     <t>גלישת זיכרון משתנה גלובאלי, במשתנה 'globalArray' מקובץ [קובץ]
 הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
 [קובץ] שורה 7 בפונקציה 'main'
 הכתובת המבוקשת ממוקמת 4 בתים מימין למשתנה הגלובאלי 'globalArray' מקובץ [קובץ], בגודל 400-בתים</t>
   </si>
   <si>
-    <t>Line 3: int main(int argc, char** argv) 
-{
- int res = -1;
- void* p = (void*)malloc(7);
- if (!p)
- {
-  res = 1;
- }
- p = (void*)malloc(7); // The memory is leaked here - no use of free()
- if (!p)
- {
-  res = 2;
- }
- return res; // The memory is leaked here - no use of free()
-}</t>
-  </si>
-  <si>
-    <t>sanitizer_leak.c:6: [#3]: Detected memory leaks, suspect variables: ['p']
-  sanitizer_leak.c:6 in function 'main'
-sanitizer_leak.c:11: Memory:[#3,#4]: Detected memory leaks, suspect variables: ['p']
-  sanitizer_leak.c:11 in function 'main'</t>
-  </si>
-  <si>
     <t>נמצאו דליפות זיכרון, משתנה חשוד ['p']
 [קובץ] שורה 6 בפונקציה 'main'
 נמצאו דליפות זיכרון, משתנה חשוד ['p']
 [קובץ] שורה 11 בפונקציה 'main'</t>
   </si>
   <si>
-    <t>Line 4: int main(int argc, char** argv) 
+    <t>[#1,#2] Heap use after free, suspect variables: ['array'], sanitizer_address-heap_use_after_free.c:8
+ Was accessed by read of size 4 at:
+  sanitizer_address-heap_use_after_free.c:8 in function 'main'
+ Accessed address is located 4 bytes inside of 400-byte region, freed by thread T0 here:
+  sanitizer_address-heap_use_after_free.c:7 in function 'main'
+ Previously allocated by thread T0 here:
+  sanitizer_address-heap_use_after_free.c:6 in function 'main'</t>
+  </si>
+  <si>
+    <t>[#4] Segmentation fault, suspect variable: 'p', sanitizer_address-segmentation_fault.c:6 at:
+  sanitizer_address-segmentation_fault.c:6 in function 'main'</t>
+  </si>
+  <si>
+    <t>[#2,#3] Stack buffer overflow, suspect variable: 'stackArray', sanitizer_address-stack_buffer_overflow.c:7
+ Was accessed by read of size 4 at:
+  sanitizer_address-stack_buffer_overflow.c:7 in function 'main'
+ Accessed address is located in stack of thread T0 at offset 692 in frame:
+  sanitizer_address-stack_buffer_overflow.c:4 in function 'main'</t>
+  </si>
+  <si>
+    <t>[#4] Heap buffer overflow, suspect variable: 'array', sanitizer_address-heap_buffer_overflow.c:8
+ Was accessed by read of size 4 at:
+  sanitizer_address-heap_buffer_overflow.c:8 in function 'main'
+ Accessed address is located 4 bytes to the right of 400-byte region, allocated at:
+  sanitizer_address-heap_buffer_overflow.c:6 in function 'main'</t>
+  </si>
+  <si>
+    <t>[#2,#3] Global variable buffer overflow, 'globalArray' from file sanitizer_address-global_buffer_overflow.c, accessed at sanitizer_address-global_buffer_overflow.c:7
+ Was accessed by read of size 4 at:
+  sanitizer_address-global_buffer_overflow.c:7 in function 'main'
+ Accessed address is located 4 bytes to the right of global variable 'globalArray' from 'sanitizer_address-global_buffer_overflow.c', of size 400</t>
+  </si>
+  <si>
+    <t>[#2] Use of uninitialized value, suspect variable: 'arr', sanitizer_memory.c:8
+ Used at:
+  sanitizer_memory.c:8 in function 'main'
+ Allocated at:
+  sanitizer_memory.c:6 in function 'main'</t>
+  </si>
+  <si>
+    <t>[#3] Detected memory leaks, suspect variable: 'p', sanitizer_leak.c:6
+  sanitizer_leak.c:6 in function 'main'
+[#2,#3] Detected memory leaks, suspect variable: 'p', sanitizer_leak.c:11
+  sanitizer_leak.c:11 in function 'main'</t>
+  </si>
+  <si>
+    <t>#include &lt;stdlib.h&gt;
+#include &lt;stdio.h&gt;
+int main(int argc, char** argv) 
 {
-     int res = -1;
-     int* arr = (int*)malloc(7*sizeof(int));
-     arr[ 2 ] = 0;  //  - OK - Write to uninitialized memory
-     if (arr[ 3 ]) // BOOM  - Read from uninitialized memory
-     {
-          res = 1;
-     }
-     free(arr);
-     return res;
-}</t>
-  </si>
-  <si>
-    <t>שימוש בערך לא מאותחל, משתנה חשוד ['arr']
-השימוש קרה ב:
-[קובץ] שורה 9 בפונקציה 'main'
-הערך הוקצה ב:
-[קובץ] שורה 7 בפונקציה 'main'</t>
-  </si>
-  <si>
-    <t>sanitizer_memory.c:9:[#2]: Use of uninitialized value, suspect variables: ['arr']
- Used at:
-  sanitizer_memory.c:9 in function 'main'
- Allocated at:
-  sanitizer_memory.c:7 in function 'main'</t>
-  </si>
-  <si>
-    <t>Line 4: int main(int argc, char** argv) 
-{
-      int res = -1;
-      int* array = (int*)malloc(100*sizeof(int));
-      array[ 0 ] = 0;
-      if (array[ argc+ 100 ])// BOOM Heap-buffer-overflow
-      {
-          res = 1; 
-      }
-      free(array);
-      return res;
-}</t>
-  </si>
-  <si>
-    <t>Line 4: int main(int argc, char** argv) 
-{
-   int res = -1;
+    int res = -1;
     int* array = (int*)malloc(100*sizeof(int));
     free(array);
     if (array[ argc ])// BOOM Heap-use-after-free 
@@ -178,40 +102,130 @@
 }</t>
   </si>
   <si>
+    <t>#include&lt;stdio.h&gt; 
+#include&lt;stdlib.h&gt; 
+int main(void) 
+{ 
+    char* p; 
+    p[ 1000 ] = 'a';
+    printf("\n %s \n", p); 
+    return 0; 
+}</t>
+  </si>
+  <si>
+    <t>#include &lt;stdlib.h&gt;
+#include &lt;stdio.h&gt;
+int main(int argc, char** argv) 
+{
+    int res = -1;
+    int* array = (int*)malloc(100*sizeof(int));
+   array[ 0 ] = 0;
+    if (array[ argc+ 100 ])// BOOM Heap-buffer-overflow
+    {
+        res = 1; 
+    }
+    free(array);
+    return res;
+}</t>
+  </si>
+  <si>
+    <t>#include &lt;stdlib.h&gt;
+#include &lt;stdio.h&gt;
+int globalArray[ 100 ] = {-1 };
+int main(int argc, char** argv) 
+{
+    int res = -1;
+    if (globalArray[ argc+ 100 ]) // BOOM Global-buffer-overflow
+    {
+        res = 1; 
+    }
+    return res;
+}</t>
+  </si>
+  <si>
+    <t>#include &lt;stdlib.h&gt;
+#include &lt;stdio.h&gt;
+int main(int argc, char** argv) 
+{
+    int res = -1;
+    int* arr = (int*)malloc(7*sizeof(int));
+    arr[ 2 ] = 0;  //  - OK - Write to uninitialized memory
+    if (arr[ 3 ]) // BOOM  - Read from uninitialized memory
+    {
+        res = 1;
+    }
+    free(arr);
+    return res;
+}</t>
+  </si>
+  <si>
+    <t>#include &lt;stdlib.h&gt;
+#include &lt;stdio.h&gt;
+int main(int argc, char** argv) 
+{
+    int res = -1;
+    void* p = (void*)malloc(7);
+    if (!p)
+    {
+        res = 1;
+    }
+    p = (void*)malloc(7); // The memory is leaked here - no use of free()
+    if (!p)
+    {
+        res = 2;
+    }
+    return res; // The memory is leaked here - no use of free()
+}</t>
+  </si>
+  <si>
+    <t>#include &lt;stdlib.h&gt;
+#include &lt;stdio.h&gt;
+int main(int argc, char** argv) 
+{
+ int res = -1;
+ int stackArray[ 100 ] = { 0 };
+ if (stackArray[ argc+ 100 ])
+ {
+  // BOOM Stack-buffer-overflow
+     res = stackArray[ argc + 100 ];  // BOOM Stack-buffer-overflow
+ }
+ return res;
+}</t>
+  </si>
+  <si>
     <t>שימוש בזיכרון שהוקצה דינאמית לאחר ששוחרר. משתנה חשוד ['array']
 הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים, ב:
-[קובץ] בשורה 9 בפונקציה 'main'
+[קובץ] בשורה 8 בפונקציה 'main'
 הגישה לזיכרון ממוקמת 4 בתים בתוך איזור זיכרון בגודל 400 בתים, שוחחר על ידי חוט T0 כאן:
+[קובץ] שורה 7 בפונקציה 'main'
+הזיכרון הוקצה לפני ששוחרר על ידי חוט T0 כאן:
+[קובץ] שורה 6 בפונקציה 'main'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">גישה לא חוקית לזיכרון (אין הרשאת גישה) - שגיאת סגמנטציה, משתנה חשוד ['p'] ב:
+[קובץ] שורה 6 בפונקציה 'main'
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">גלישת זיכרון מחסנית, משתנה חשוד ['stackArray']
+הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
+[קובץ] שורה 7 בפונקציה 'main'
+הכתובת המבוקשת ממוקמת במחסנית של חוט T0 בהיסט של 692 בתים במסגרת:
+[קובץ] שורה 4 בפונקציה 'main'   </t>
+  </si>
+  <si>
+    <t>גלישת זיכרון ערימה, משתנה חשוד ['array']
+הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
 [קובץ] שורה 8 בפונקציה 'main'
-הזיכרון הוקצה לפני ששוחרר על ידי חוט T0 כאן:
-[קובץ] שורה 7 בפונקציה 'main'</t>
-  </si>
-  <si>
-    <t>program.c:9: [#1]: Segmentation fault, suspect variables: ['p'] at:
-  program.c:9 in function 'main'</t>
-  </si>
-  <si>
-    <t>program.c:9:[#1,#3]: Heap use after free, suspect variables: ['array']
- Was accessed by read of size 4 at:
-  sanitizer_address-heap_use_after_free.c:9 in function 'main'
- Accessed address is located 4 bytes inside of 400-byte region, freed by thread T0 here:
-  program.c:8 in function 'main'
- previously allocated by thread T0 here:
-  program.c:7 in function 'main'</t>
-  </si>
-  <si>
-    <t>program.c:9: Memory:[#4]: Heap buffer overflow, suspect variables: ['array']
- Was accessed by read of size 4 at:
-  program.c:9 in function 'main'
- Accessed address is located 4 bytes to the right of 400-byte region, allocated at:
-  program.c:7 in function 'main'</t>
-  </si>
-  <si>
-    <t>program.c:7: Memory:[#2,#3]: Global variable buffer overflow, 'globalArray' from file sanitizer_address-global_buffer_overflow.c
- Was accessed by read of size 4 at:
-  sanitizer_address-global_buffer_overflow.c:7 in function 'main'
- Accessed address is located 4 bytes to the right of global variable 'globalArray' from 'sanitizer_address-global_buffer_overflow.c',
- of size 400</t>
+הכתובת המבוקשת ממוקמת 4 בתים מימין לאיזור זיכרון בגודל 400-בתים, שהוקצה ב:
+[קובץ] שורה 6 בפונקציה 'main'</t>
+  </si>
+  <si>
+    <t>שימוש בערך לא מאותחל, משתנה חשוד ['arr']
+השימוש קרה ב:
+[קובץ] שורה 8 בפונקציה 'main'
+הערך הוקצה ב:
+[קובץ] שורה 6 בפונקציה 'main'</t>
   </si>
 </sst>
 </file>
@@ -568,7 +582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -577,84 +593,84 @@
     <col min="3" max="3" width="63.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="145" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="203" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="203" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="145" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="174" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed memory sanitizer test case so it would trigger the memory sanitizer
- Updated the error guide also
</commit_message>
<xml_diff>
--- a/vera/error_guide.xlsx
+++ b/vera/error_guide.xlsx
@@ -24,30 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>גלישת זיכרון משתנה גלובאלי, במשתנה 'globalArray' מקובץ [קובץ]
 הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
 [קובץ] שורה 7 בפונקציה 'main'
 הכתובת המבוקשת ממוקמת 4 בתים מימין למשתנה הגלובאלי 'globalArray' מקובץ [קובץ], בגודל 400-בתים</t>
-  </si>
-  <si>
-    <t>נמצאו דליפות זיכרון, משתנה חשוד ['p']
-[קובץ] שורה 6 בפונקציה 'main'
-נמצאו דליפות זיכרון, משתנה חשוד ['p']
-[קובץ] שורה 11 בפונקציה 'main'</t>
-  </si>
-  <si>
-    <t>[#1,#2] Heap use after free, suspect variables: ['array'], sanitizer_address-heap_use_after_free.c:8
- Was accessed by read of size 4 at:
-  sanitizer_address-heap_use_after_free.c:8 in function 'main'
- Accessed address is located 4 bytes inside of 400-byte region, freed by thread T0 here:
-  sanitizer_address-heap_use_after_free.c:7 in function 'main'
- Previously allocated by thread T0 here:
-  sanitizer_address-heap_use_after_free.c:6 in function 'main'</t>
   </si>
   <si>
     <t>[#4] Segmentation fault, suspect variable: 'p', sanitizer_address-segmentation_fault.c:6 at:
@@ -72,13 +54,6 @@
  Was accessed by read of size 4 at:
   sanitizer_address-global_buffer_overflow.c:7 in function 'main'
  Accessed address is located 4 bytes to the right of global variable 'globalArray' from 'sanitizer_address-global_buffer_overflow.c', of size 400</t>
-  </si>
-  <si>
-    <t>[#2] Use of uninitialized value, suspect variable: 'arr', sanitizer_memory.c:8
- Used at:
-  sanitizer_memory.c:8 in function 'main'
- Allocated at:
-  sanitizer_memory.c:6 in function 'main'</t>
   </si>
   <si>
     <t>[#3] Detected memory leaks, suspect variable: 'p', sanitizer_leak.c:6
@@ -139,22 +114,6 @@
     {
         res = 1; 
     }
-    return res;
-}</t>
-  </si>
-  <si>
-    <t>#include &lt;stdlib.h&gt;
-#include &lt;stdio.h&gt;
-int main(int argc, char** argv) 
-{
-    int res = -1;
-    int* arr = (int*)malloc(7*sizeof(int));
-    arr[ 2 ] = 0;  //  - OK - Write to uninitialized memory
-    if (arr[ 3 ]) // BOOM  - Read from uninitialized memory
-    {
-        res = 1;
-    }
-    free(arr);
     return res;
 }</t>
   </si>
@@ -193,7 +152,60 @@
 }</t>
   </si>
   <si>
-    <t>שימוש בזיכרון שהוקצה דינאמית לאחר ששוחרר. משתנה חשוד ['array']
+    <t xml:space="preserve"> - גישה לכתובת זיכרון לא חוקית / מחוץ לטווח הזיכרון של התכנית</t>
+  </si>
+  <si>
+    <t> גישה לזיכרון שהוקצה דינמית, לאחר ששוחרר (free)</t>
+  </si>
+  <si>
+    <t>גלישת זיכרון מחסנית</t>
+  </si>
+  <si>
+    <t>גלישת זיכרון ערימה</t>
+  </si>
+  <si>
+    <t>גלישת זיכרון משתנה גלובאלי</t>
+  </si>
+  <si>
+    <t>Memory leak</t>
+  </si>
+  <si>
+    <t>Uninitialized memory use</t>
+  </si>
+  <si>
+    <t>Heap use after free</t>
+  </si>
+  <si>
+    <t>Heap buffer overflow</t>
+  </si>
+  <si>
+    <t>Global buffer overflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stack buffer overflow  </t>
+  </si>
+  <si>
+    <t> Segmentation fault </t>
+  </si>
+  <si>
+    <t>דליפת זיכרון, 
+זיכרון שהוקצה לא שוחרר (free)</t>
+  </si>
+  <si>
+    <t>גישה לתא בזיכרון שהוקצה דינמית,
+ אך לא אותחל</t>
+  </si>
+  <si>
+    <t>[#1,#2] Heap use after free, suspect variables: 'array', sanitizer_address-heap_use_after_free.c:8
+ Was accessed by read of size 4 at:
+  sanitizer_address-heap_use_after_free.c:8 in function 'main'
+ Accessed address is located 4 bytes inside of 400-byte region, freed by thread T0 here:
+  sanitizer_address-heap_use_after_free.c:7 in function 'main'
+ Previously allocated by thread T0 here:
+  sanitizer_address-heap_use_after_free.c:6 in function 'main'</t>
+  </si>
+  <si>
+    <t>שימוש בזיכרון שהוקצה דינאמית לאחר ששוחרר. משתנה חשוד 'array'
 הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים, ב:
 [קובץ] בשורה 8 בפונקציה 'main'
 הגישה לזיכרון ממוקמת 4 בתים בתוך איזור זיכרון בגודל 400 בתים, שוחחר על ידי חוט T0 כאן:
@@ -202,39 +214,80 @@
 [קובץ] שורה 6 בפונקציה 'main'</t>
   </si>
   <si>
-    <t xml:space="preserve">גישה לא חוקית לזיכרון (אין הרשאת גישה) - שגיאת סגמנטציה, משתנה חשוד ['p'] ב:
-[קובץ] שורה 6 בפונקציה 'main'
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">גלישת זיכרון מחסנית, משתנה חשוד ['stackArray']
+    <t>גלישת זיכרון ערימה, משתנה חשוד 'array'
+הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
+[קובץ] שורה 8 בפונקציה 'main'
+הכתובת המבוקשת ממוקמת 4 בתים מימין לאיזור זיכרון בגודל 400-בתים, שהוקצה ב:
+[קובץ] שורה 6 בפונקציה 'main'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">גלישת זיכרון מחסנית, משתנה חשוד 'stackArray'
 הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
 [קובץ] שורה 7 בפונקציה 'main'
 הכתובת המבוקשת ממוקמת במחסנית של חוט T0 בהיסט של 692 בתים במסגרת:
 [קובץ] שורה 4 בפונקציה 'main'   </t>
   </si>
   <si>
-    <t>גלישת זיכרון ערימה, משתנה חשוד ['array']
-הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
-[קובץ] שורה 8 בפונקציה 'main'
-הכתובת המבוקשת ממוקמת 4 בתים מימין לאיזור זיכרון בגודל 400-בתים, שהוקצה ב:
-[קובץ] שורה 6 בפונקציה 'main'</t>
-  </si>
-  <si>
-    <t>שימוש בערך לא מאותחל, משתנה חשוד ['arr']
+    <t xml:space="preserve">גישה לא חוקית לזיכרון (אין הרשאת גישה) - שגיאת סגמנטציה, משתנה חשוד 'p' ב:
+[קובץ] שורה 6 בפונקציה 'main'
+</t>
+  </si>
+  <si>
+    <t>נמצאו דליפות זיכרון, משתנה חשוד 'p'
+[קובץ] שורה 6 בפונקציה 'main'
+נמצאו דליפות זיכרון, משתנה חשוד 'p'
+[קובץ] שורה 11 בפונקציה 'main'</t>
+  </si>
+  <si>
+    <t>#include &lt;stdlib.h&gt;
+#include &lt;stdio.h&gt;
+int main(int argc, char** argv) 
+{
+    int* arr = (int*)malloc(7*sizeof(int));
+    arr[ 2 ] = 0;  //  - OK - Write to uninitialized memory
+    if (arr[ argc ]) // BOOM  - Read from uninitialized memory
+    {
+        printf("xx\n");
+    }
+    free(arr);
+    return 0
+}</t>
+  </si>
+  <si>
+    <t>שימוש בערך לא מאותחל, משתנה חשוד 'arr'
 השימוש קרה ב:
-[קובץ] שורה 8 בפונקציה 'main'
+[קובץ] שורה 7 בפונקציה 'main'
 הערך הוקצה ב:
-[קובץ] שורה 6 בפונקציה 'main'</t>
+[קובץ] שורה 5 בפונקציה 'main'</t>
+  </si>
+  <si>
+    <t>[#2] Use of uninitialized value, suspect variable: 'arr', sanitizer_memory.c:7
+ Used at:
+  sanitizer_memory.c:7 in function 'main'
+ Allocated at:
+  sanitizer_memory.c:5 in function 'main'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -261,9 +314,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -580,100 +641,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="94.26953125" customWidth="1"/>
     <col min="2" max="2" width="62.6328125" customWidth="1"/>
     <col min="3" max="3" width="63.6328125" customWidth="1"/>
+    <col min="4" max="4" width="28" style="4" customWidth="1"/>
+    <col min="5" max="5" width="46.453125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="132" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="190" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="204.5" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="175.5" x14ac:dyDescent="0.5">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="190" x14ac:dyDescent="0.5">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="248" x14ac:dyDescent="0.5">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="203" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="174" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="203" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="246.5" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="190" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added additional sanitizer errors handling
</commit_message>
<xml_diff>
--- a/vera/error_guide.xlsx
+++ b/vera/error_guide.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>גלישת זיכרון משתנה גלובאלי, במשתנה 'globalArray' מקובץ [קובץ]
 הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
@@ -205,15 +205,6 @@
   sanitizer_address-heap_use_after_free.c:6 in function 'main'</t>
   </si>
   <si>
-    <t>שימוש בזיכרון שהוקצה דינאמית לאחר ששוחרר. משתנה חשוד 'array'
-הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים, ב:
-[קובץ] בשורה 8 בפונקציה 'main'
-הגישה לזיכרון ממוקמת 4 בתים בתוך איזור זיכרון בגודל 400 בתים, שוחחר על ידי חוט T0 כאן:
-[קובץ] שורה 7 בפונקציה 'main'
-הזיכרון הוקצה לפני ששוחרר על ידי חוט T0 כאן:
-[קובץ] שורה 6 בפונקציה 'main'</t>
-  </si>
-  <si>
     <t>גלישת זיכרון ערימה, משתנה חשוד 'array'
 הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
 [קובץ] שורה 8 בפונקציה 'main'
@@ -239,21 +230,6 @@
 [קובץ] שורה 11 בפונקציה 'main'</t>
   </si>
   <si>
-    <t>#include &lt;stdlib.h&gt;
-#include &lt;stdio.h&gt;
-int main(int argc, char** argv) 
-{
-    int* arr = (int*)malloc(7*sizeof(int));
-    arr[ 2 ] = 0;  //  - OK - Write to uninitialized memory
-    if (arr[ argc ]) // BOOM  - Read from uninitialized memory
-    {
-        printf("xx\n");
-    }
-    free(arr);
-    return 0
-}</t>
-  </si>
-  <si>
     <t>שימוש בערך לא מאותחל, משתנה חשוד 'arr'
 השימוש קרה ב:
 [קובץ] שורה 7 בפונקציה 'main'
@@ -266,6 +242,108 @@
   sanitizer_memory.c:7 in function 'main'
  Allocated at:
   sanitizer_memory.c:5 in function 'main'</t>
+  </si>
+  <si>
+    <t>#include &lt;stdlib.h&gt;
+#include &lt;stdio.h&gt;
+int main(int argc, char** argv) 
+{
+    int* arr = (int*)malloc(7*sizeof(int)), result = 0;
+    if (!arr) 
+    {
+        result = -1;
+    }
+    arr[ 2 ] = 0;  //  - OK - Write to uninitialized memory
+    if (arr[ argc ]) // BOOM  - Read from uninitialized memory
+    {
+        printf(Read from uninitialized memory");
+    }
+    free(arr);
+    return result;
+}</t>
+  </si>
+  <si>
+    <t>[#1] Memory use after function return, suspect variable: 'ptr', sanitizer_address-stack_use_after_return.c:10
+ Was accessed by read of size 4 at:
+  sanitizer_address-stack_use_after_return.c:10 in function 'main'
+ Accessed address is located in stack of thread T0 at offset 36 in frame:
+  sanitizer_address-stack_use_after_return.c:3 in function 'functionThatEscapesLocalObject'</t>
+  </si>
+  <si>
+    <t>שימוש בזיכרון שהוקצה דינאמית לאחר ששוחרר. משתנה חשוד 'array'
+הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים, ב:
+[קובץ] בשורה 8 בפונקציה 'main'
+הכתובת המבוקשת ממוקמת 4 בתים בתוך איזור זיכרון בגודל 400 בתים, שוחחר על ידי חוט T0 כאן:
+[קובץ] שורה 7 בפונקציה 'main'
+הזיכרון הוקצה לפני ששוחרר על ידי חוט T0 כאן:
+[קובץ] שורה 6 בפונקציה 'main'</t>
+  </si>
+  <si>
+    <t>שימוש בזיכרון לאחר חזרה מפונקציה' משתנה חשוד 'ptr', [קובץ] שורה 10
+הגישה לזיכרון היתה מסוג קריאה בגודל 4 בתים ב:
+[קובץ] שורה 10
+הכתובת המבוקשת ממוקמת במחסנית של חוט T0 בהיסט של 36 בתים בתוך המסגרת:
+[קובץ] שורה 3</t>
+  </si>
+  <si>
+    <t>שימוש בזיכרון מחסנית של פונקציה שהסתיימה</t>
+  </si>
+  <si>
+    <t>[#2] Double free of memory, suspect variable: 'p', sanitizer_address-heap_double_free.c:11
+ Attempted double free in thread T0:
+  sanitizer_address-heap_double_free.c:11 in function 'main'
+ Freed address is located 0 bytes inside of 8-byte region, already freed by thread T0 here:
+  sanitizer_address-heap_double_free.c:10 in function 'main'
+ Previously allocated by thread T0 here:
+  sanitizer_address-heap_double_free.c:5 in function 'main'</t>
+  </si>
+  <si>
+    <t>שחרור כפול של זיכרון, משתנה חשוד 'p', [קובץ] שורה 11
+השחרור השנימחוט T0 ב:
+[קובץ] שורה 11
+הכתובת המבוקשת ממוקמת 0 בתים בתוך איזור זיכרון של 8 בתים,
+ כבר שוחרר על ידי חוט T0 ב:
+[קובץ] שורה 10
+הוקצה לפני כן על ידי חוט T0 ב:
+[קובץ] שורה 5</t>
+  </si>
+  <si>
+    <t>Double free of memory</t>
+  </si>
+  <si>
+    <t>Memory use after
+ function return</t>
+  </si>
+  <si>
+    <t>שחרור כפול של זיכרון</t>
+  </si>
+  <si>
+    <t>int* ptr = 0;
+void functionThatEscapesLocalObject() 
+{
+    int local[ 100 ] = { 0 };
+    ptr = &amp;local[ 0 ];
+}
+int main(int argc, char **argv) 
+{
+    functionThatEscapesLocalObject();
+    return ptr[ argc ];
+}</t>
+  </si>
+  <si>
+    <t>#include&lt;stdio.h&gt; 
+#include&lt;stdlib.h&gt; 
+int main(int argc, char *argv[]) 
+{ 
+    char* p = (char*)malloc(8); 
+    if (!p) 
+    {
+        printf("malloc error");
+    }
+    free(p); 
+    free(p); 
+    return 0; 
+}</t>
   </si>
 </sst>
 </file>
@@ -643,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -652,7 +730,7 @@
     <col min="1" max="1" width="94.26953125" customWidth="1"/>
     <col min="2" max="2" width="62.6328125" customWidth="1"/>
     <col min="3" max="3" width="63.6328125" customWidth="1"/>
-    <col min="4" max="4" width="28" style="4" customWidth="1"/>
+    <col min="4" max="4" width="31.26953125" style="4" customWidth="1"/>
     <col min="5" max="5" width="46.453125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -661,7 +739,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -678,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -695,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -729,7 +807,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -746,7 +824,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
@@ -758,15 +836,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="190" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" ht="248" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>18</v>
@@ -775,19 +853,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
+    <row r="8" spans="1:5" ht="190" x14ac:dyDescent="0.5">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
+    <row r="9" spans="1:5" ht="161" x14ac:dyDescent="0.5">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>